<commit_message>
correlation and simulation project were added
</commit_message>
<xml_diff>
--- a/projects/probability_of_default/data/output/descriptive_summary.xlsx
+++ b/projects/probability_of_default/data/output/descriptive_summary.xlsx
@@ -524,9 +524,11 @@
       <c r="I2" t="n">
         <v>29465</v>
       </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>32581</v>
+      </c>
       <c r="K2" t="n">
-        <v>32572</v>
+        <v>32581</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
@@ -555,11 +557,13 @@
         <v>9589.371105859243</v>
       </c>
       <c r="I3" t="n">
-        <v>11.01169483450866</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
+        <v>11.01169489224504</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.2181639605905282</v>
+      </c>
       <c r="K3" t="n">
-        <v>0.1702505220307043</v>
+        <v>0.1702034928332464</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
@@ -588,11 +592,13 @@
         <v>6322.086645792259</v>
       </c>
       <c r="I4" t="n">
-        <v>3.240459475983925</v>
-      </c>
-      <c r="J4" t="inlineStr"/>
+        <v>3.240459464955947</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.4130056685601487</v>
+      </c>
       <c r="K4" t="n">
-        <v>0.1067590146706945</v>
+        <v>0.1067817563449238</v>
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
@@ -621,11 +627,13 @@
         <v>500</v>
       </c>
       <c r="I5" t="n">
-        <v>5.420000076293945</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
+        <v>5.42</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
       <c r="K5" t="n">
-        <v>0.009999999776482582</v>
+        <v>0</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
@@ -654,11 +662,13 @@
         <v>5000</v>
       </c>
       <c r="I6" t="n">
-        <v>7.900000095367432</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
+        <v>7.9</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
       <c r="K6" t="n">
-        <v>0.09000000357627869</v>
+        <v>0.09</v>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
@@ -687,11 +697,13 @@
         <v>8000</v>
       </c>
       <c r="I7" t="n">
-        <v>10.98999977111816</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
+        <v>10.99</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
       <c r="K7" t="n">
-        <v>0.1500000059604645</v>
+        <v>0.15</v>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
@@ -720,11 +732,13 @@
         <v>12200</v>
       </c>
       <c r="I8" t="n">
-        <v>13.47000026702881</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
+        <v>13.47</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
       <c r="K8" t="n">
-        <v>0.2300000041723251</v>
+        <v>0.23</v>
       </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
@@ -753,11 +767,13 @@
         <v>35000</v>
       </c>
       <c r="I9" t="n">
-        <v>23.21999931335449</v>
-      </c>
-      <c r="J9" t="inlineStr"/>
+        <v>23.22</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
       <c r="K9" t="n">
-        <v>0.8299999833106995</v>
+        <v>0.83</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
@@ -786,11 +802,13 @@
         <v>1.1924774277662</v>
       </c>
       <c r="I10" t="n">
-        <v>0.208550355322592</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
+        <v>0.2085503016908977</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.364888487327168</v>
+      </c>
       <c r="K10" t="n">
-        <v>1.065441677161143</v>
+        <v>1.064668636768324</v>
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
@@ -819,11 +837,13 @@
         <v>1.423565307276444</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.6716090778773895</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
+        <v>-0.6716091079813706</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-0.137087836131323</v>
+      </c>
       <c r="K11" t="n">
-        <v>1.224790914120473</v>
+        <v>1.223686678285682</v>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
@@ -852,11 +872,13 @@
         <v>2000</v>
       </c>
       <c r="I12" t="n">
-        <v>6.03000020980835</v>
-      </c>
-      <c r="J12" t="inlineStr"/>
+        <v>6.03</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
       <c r="K12" t="n">
-        <v>0.03999999910593033</v>
+        <v>0.04</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
@@ -885,11 +907,13 @@
         <v>24000</v>
       </c>
       <c r="I13" t="n">
-        <v>16.31999969482422</v>
-      </c>
-      <c r="J13" t="inlineStr"/>
+        <v>16.32</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
       <c r="K13" t="n">
-        <v>0.3799999952316284</v>
+        <v>0.38</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
@@ -930,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
         <v>0</v>
@@ -973,7 +997,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.02762346152665664</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
@@ -1016,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="K16" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L16" t="n">
         <v>2</v>
@@ -1049,9 +1073,11 @@
       <c r="I17" t="n">
         <v>1.068107179030723</v>
       </c>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>0.006138547005923698</v>
+      </c>
       <c r="K17" t="n">
-        <v>0.2332647862251005</v>
+        <v>0.2363340597280624</v>
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
@@ -1082,9 +1108,11 @@
       <c r="I18" t="n">
         <v>0</v>
       </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>25473</v>
+      </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
@@ -1115,9 +1143,11 @@
       <c r="I19" t="n">
         <v>0</v>
       </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>78.18360394094718</v>
+      </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>0.02762346152665664</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
@@ -1146,11 +1176,13 @@
         <v>34500</v>
       </c>
       <c r="I20" t="n">
-        <v>17.79999923706055</v>
-      </c>
-      <c r="J20" t="inlineStr"/>
+        <v>17.8</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
       <c r="K20" t="n">
-        <v>0.8199999835342169</v>
+        <v>0.83</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
@@ -1179,11 +1211,13 @@
         <v>7200</v>
       </c>
       <c r="I21" t="n">
-        <v>5.570000171661377</v>
-      </c>
-      <c r="J21" t="inlineStr"/>
+        <v>5.57</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
       <c r="K21" t="n">
-        <v>0.1400000005960464</v>
+        <v>0.14</v>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
@@ -1212,11 +1246,13 @@
         <v>39968779.55690482</v>
       </c>
       <c r="I22" t="n">
-        <v>10.50057761549401</v>
-      </c>
-      <c r="J22" t="inlineStr"/>
+        <v>10.50057754402258</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.1705736822628154</v>
+      </c>
       <c r="K22" t="n">
-        <v>0.01139748721345757</v>
+        <v>0.01140234348810668</v>
       </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
@@ -1245,11 +1281,13 @@
         <v>312431300</v>
       </c>
       <c r="I23" t="n">
-        <v>324459.5882987976</v>
-      </c>
-      <c r="J23" t="inlineStr"/>
+        <v>324459.59</v>
+      </c>
+      <c r="J23" t="n">
+        <v>7108</v>
+      </c>
       <c r="K23" t="n">
-        <v>5545.400003584102</v>
+        <v>5545.400000000001</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">

</xml_diff>